<commit_message>
Ordena por Apellido del Alumno
</commit_message>
<xml_diff>
--- a/calificaciones_alumnos_modificado.xlsx
+++ b/calificaciones_alumnos_modificado.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,19 +474,14 @@
           <t>Promedio</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Mat_Fisica</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Alberto</t>
+          <t>Pedro</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -496,32 +491,29 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Alberto Fernández</t>
+          <t>Pedro Fernández</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>67.7</v>
+        <v>99</v>
       </c>
       <c r="F2" t="n">
-        <v>68.2</v>
+        <v>63.3</v>
       </c>
       <c r="G2" t="n">
-        <v>61.1</v>
+        <v>84.90000000000001</v>
       </c>
       <c r="H2" t="n">
-        <v>65.7</v>
-      </c>
-      <c r="I2" t="n">
-        <v>41.3</v>
+        <v>82.40000000000001</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Alberto</t>
+          <t>María</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -531,23 +523,20 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Alberto Fernández</t>
+          <t>María Fernández</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>86.59999999999999</v>
+        <v>72</v>
       </c>
       <c r="F3" t="n">
-        <v>96.90000000000001</v>
+        <v>79.7</v>
       </c>
       <c r="G3" t="n">
-        <v>90.2</v>
+        <v>95.8</v>
       </c>
       <c r="H3" t="n">
-        <v>91.2</v>
-      </c>
-      <c r="I3" t="n">
-        <v>19</v>
+        <v>82.5</v>
       </c>
     </row>
     <row r="4">
@@ -581,83 +570,74 @@
       <c r="H4" t="n">
         <v>91.90000000000001</v>
       </c>
-      <c r="I4" t="n">
-        <v>73.8</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Alberto</t>
+          <t>Ángel</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>García</t>
+          <t>Fernández</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Alberto García</t>
+          <t>Ángel Fernández</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>62.3</v>
+        <v>81.5</v>
       </c>
       <c r="F5" t="n">
-        <v>57.6</v>
+        <v>85</v>
       </c>
       <c r="G5" t="n">
-        <v>81.7</v>
+        <v>96.3</v>
       </c>
       <c r="H5" t="n">
-        <v>67.2</v>
-      </c>
-      <c r="I5" t="n">
-        <v>37.6</v>
+        <v>87.59999999999999</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Alberto</t>
+          <t>María</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>García</t>
+          <t>Fernández</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Alberto García</t>
+          <t>María Fernández</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>62.3</v>
+        <v>70.59999999999999</v>
       </c>
       <c r="F6" t="n">
-        <v>81</v>
+        <v>83.7</v>
       </c>
       <c r="G6" t="n">
-        <v>57.6</v>
+        <v>73.59999999999999</v>
       </c>
       <c r="H6" t="n">
-        <v>67</v>
-      </c>
-      <c r="I6" t="n">
-        <v>79.8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -666,68 +646,62 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Martínez</t>
+          <t>Fernández</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Alberto Martínez</t>
+          <t>Alberto Fernández</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>76.5</v>
+        <v>67.7</v>
       </c>
       <c r="F7" t="n">
-        <v>86.40000000000001</v>
+        <v>68.2</v>
       </c>
       <c r="G7" t="n">
-        <v>67.40000000000001</v>
+        <v>61.1</v>
       </c>
       <c r="H7" t="n">
-        <v>76.8</v>
-      </c>
-      <c r="I7" t="n">
-        <v>65.59999999999999</v>
+        <v>65.7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Alberto</t>
+          <t>Victor</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Martínez</t>
+          <t>Fernández</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Alberto Martínez</t>
+          <t>Victor Fernández</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>92.09999999999999</v>
+        <v>60.8</v>
       </c>
       <c r="F8" t="n">
-        <v>95.09999999999999</v>
+        <v>80.09999999999999</v>
       </c>
       <c r="G8" t="n">
-        <v>63</v>
+        <v>98.5</v>
       </c>
       <c r="H8" t="n">
-        <v>83.40000000000001</v>
-      </c>
-      <c r="I8" t="n">
-        <v>67.09999999999999</v>
+        <v>79.8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -736,142 +710,130 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Pérez</t>
+          <t>Fernández</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Alberto Pérez</t>
+          <t>Alberto Fernández</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>61.1</v>
+        <v>86.59999999999999</v>
       </c>
       <c r="F9" t="n">
-        <v>60.8</v>
+        <v>96.90000000000001</v>
       </c>
       <c r="G9" t="n">
-        <v>70.2</v>
+        <v>90.2</v>
       </c>
       <c r="H9" t="n">
-        <v>64</v>
-      </c>
-      <c r="I9" t="n">
-        <v>47.4</v>
+        <v>91.2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Alberto</t>
+          <t>Pedro</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Pérez</t>
+          <t>García</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Alberto Pérez</t>
+          <t>Pedro García</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>53.8</v>
+        <v>89.3</v>
       </c>
       <c r="F10" t="n">
-        <v>99.3</v>
+        <v>85.40000000000001</v>
       </c>
       <c r="G10" t="n">
-        <v>91.59999999999999</v>
+        <v>78</v>
       </c>
       <c r="H10" t="n">
-        <v>81.59999999999999</v>
-      </c>
-      <c r="I10" t="n">
-        <v>86.8</v>
+        <v>84.2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Alberto</t>
+          <t>María</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Pérez</t>
+          <t>García</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Alberto Pérez</t>
+          <t>María García</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>83.40000000000001</v>
+        <v>59.2</v>
       </c>
       <c r="F11" t="n">
-        <v>95.90000000000001</v>
+        <v>67.59999999999999</v>
       </c>
       <c r="G11" t="n">
-        <v>75.8</v>
+        <v>94.09999999999999</v>
       </c>
       <c r="H11" t="n">
-        <v>85</v>
-      </c>
-      <c r="I11" t="n">
-        <v>12.6</v>
+        <v>73.59999999999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Alberto</t>
+          <t>Sofía</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Rodríguez</t>
+          <t>García</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Alberto Rodríguez</t>
+          <t>Sofía García</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>75.09999999999999</v>
+        <v>87</v>
       </c>
       <c r="F12" t="n">
-        <v>94</v>
+        <v>62.6</v>
       </c>
       <c r="G12" t="n">
-        <v>62.9</v>
+        <v>58.4</v>
       </c>
       <c r="H12" t="n">
-        <v>77.3</v>
-      </c>
-      <c r="I12" t="n">
-        <v>72.2</v>
+        <v>69.3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ana</t>
+          <t>Victor</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -881,28 +843,25 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Ana García</t>
+          <t>Victor García</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>68.7</v>
+        <v>67.8</v>
       </c>
       <c r="F13" t="n">
-        <v>58.5</v>
+        <v>58.6</v>
       </c>
       <c r="G13" t="n">
-        <v>63.4</v>
+        <v>76.59999999999999</v>
       </c>
       <c r="H13" t="n">
-        <v>63.5</v>
-      </c>
-      <c r="I13" t="n">
-        <v>7.6</v>
+        <v>67.7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -920,129 +879,117 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>70.5</v>
+        <v>68.7</v>
       </c>
       <c r="F14" t="n">
-        <v>63.3</v>
+        <v>58.5</v>
       </c>
       <c r="G14" t="n">
-        <v>71.40000000000001</v>
+        <v>63.4</v>
       </c>
       <c r="H14" t="n">
-        <v>68.40000000000001</v>
-      </c>
-      <c r="I14" t="n">
-        <v>8.300000000000001</v>
+        <v>63.5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Ana</t>
+          <t>Luis</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>López</t>
+          <t>García</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Ana López</t>
+          <t>Luis García</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>68.59999999999999</v>
+        <v>69.5</v>
       </c>
       <c r="F15" t="n">
-        <v>98.09999999999999</v>
+        <v>61.9</v>
       </c>
       <c r="G15" t="n">
-        <v>66.8</v>
+        <v>86.2</v>
       </c>
       <c r="H15" t="n">
-        <v>77.8</v>
-      </c>
-      <c r="I15" t="n">
-        <v>55.9</v>
+        <v>72.5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Ana</t>
+          <t>Alberto</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>López</t>
+          <t>García</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Ana López</t>
+          <t>Alberto García</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>72.2</v>
+        <v>62.3</v>
       </c>
       <c r="F16" t="n">
-        <v>75.8</v>
+        <v>57.6</v>
       </c>
       <c r="G16" t="n">
-        <v>98.40000000000001</v>
+        <v>81.7</v>
       </c>
       <c r="H16" t="n">
-        <v>82.09999999999999</v>
-      </c>
-      <c r="I16" t="n">
-        <v>57</v>
+        <v>67.2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Ana</t>
+          <t>Victor</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>López</t>
+          <t>García</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Ana López</t>
+          <t>Victor García</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>76.7</v>
+        <v>60.9</v>
       </c>
       <c r="F17" t="n">
-        <v>74.09999999999999</v>
+        <v>70.09999999999999</v>
       </c>
       <c r="G17" t="n">
-        <v>89.3</v>
+        <v>86.3</v>
       </c>
       <c r="H17" t="n">
-        <v>80</v>
-      </c>
-      <c r="I17" t="n">
-        <v>28</v>
+        <v>72.40000000000001</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1051,72 +998,66 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>López</t>
+          <t>García</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Ana López</t>
+          <t>Ana García</t>
         </is>
       </c>
       <c r="E18" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="F18" t="n">
         <v>63.3</v>
       </c>
-      <c r="F18" t="n">
-        <v>52.4</v>
-      </c>
       <c r="G18" t="n">
-        <v>93.40000000000001</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="H18" t="n">
-        <v>69.7</v>
-      </c>
-      <c r="I18" t="n">
-        <v>84.59999999999999</v>
+        <v>68.40000000000001</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Ana</t>
+          <t>Alberto</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Rodríguez</t>
+          <t>García</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Ana Rodríguez</t>
+          <t>Alberto García</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>61.6</v>
+        <v>62.3</v>
       </c>
       <c r="F19" t="n">
-        <v>63.7</v>
+        <v>81</v>
       </c>
       <c r="G19" t="n">
-        <v>69.90000000000001</v>
+        <v>57.6</v>
       </c>
       <c r="H19" t="n">
-        <v>65.09999999999999</v>
-      </c>
-      <c r="I19" t="n">
-        <v>42.9</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Juan</t>
+          <t>Ángel</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1126,343 +1067,313 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Juan González</t>
+          <t>Ángel González</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>78.59999999999999</v>
+        <v>74.90000000000001</v>
       </c>
       <c r="F20" t="n">
-        <v>98.09999999999999</v>
+        <v>70.3</v>
       </c>
       <c r="G20" t="n">
-        <v>69.90000000000001</v>
+        <v>83.09999999999999</v>
       </c>
       <c r="H20" t="n">
-        <v>82.2</v>
-      </c>
-      <c r="I20" t="n">
-        <v>94.3</v>
+        <v>76.09999999999999</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Juan</t>
+          <t>Pedro</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Martínez</t>
+          <t>González</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Juan Martínez</t>
+          <t>Pedro González</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>93.2</v>
+        <v>55.6</v>
       </c>
       <c r="F21" t="n">
-        <v>70.40000000000001</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="G21" t="n">
-        <v>83.7</v>
+        <v>65.59999999999999</v>
       </c>
       <c r="H21" t="n">
-        <v>82.40000000000001</v>
-      </c>
-      <c r="I21" t="n">
-        <v>21.8</v>
+        <v>66.59999999999999</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Luis</t>
+          <t>Juan</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>García</t>
+          <t>González</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Luis García</t>
+          <t>Juan González</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>69.5</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="F22" t="n">
-        <v>61.9</v>
+        <v>98.09999999999999</v>
       </c>
       <c r="G22" t="n">
-        <v>86.2</v>
+        <v>69.90000000000001</v>
       </c>
       <c r="H22" t="n">
-        <v>72.5</v>
-      </c>
-      <c r="I22" t="n">
-        <v>95.09999999999999</v>
+        <v>82.2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Luis</t>
+          <t>Sofía</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Martínez</t>
+          <t>González</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Luis Martínez</t>
+          <t>Sofía González</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>50.5</v>
+        <v>65.59999999999999</v>
       </c>
       <c r="F23" t="n">
-        <v>78.2</v>
+        <v>74.09999999999999</v>
       </c>
       <c r="G23" t="n">
-        <v>77.09999999999999</v>
+        <v>80.90000000000001</v>
       </c>
       <c r="H23" t="n">
-        <v>68.59999999999999</v>
-      </c>
-      <c r="I23" t="n">
-        <v>25.6</v>
+        <v>73.5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Luis</t>
+          <t>Sofía</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Martínez</t>
+          <t>González</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Luis Martínez</t>
+          <t>Sofía González</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>93.7</v>
+        <v>59.2</v>
       </c>
       <c r="F24" t="n">
-        <v>84.3</v>
+        <v>95.7</v>
       </c>
       <c r="G24" t="n">
-        <v>51</v>
+        <v>52.9</v>
       </c>
       <c r="H24" t="n">
-        <v>76.3</v>
-      </c>
-      <c r="I24" t="n">
-        <v>79.7</v>
+        <v>69.3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>María</t>
+          <t>Victor</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Fernández</t>
+          <t>González</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>María Fernández</t>
+          <t>Victor González</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>70.59999999999999</v>
+        <v>82.5</v>
       </c>
       <c r="F25" t="n">
-        <v>83.7</v>
+        <v>64.40000000000001</v>
       </c>
       <c r="G25" t="n">
-        <v>73.59999999999999</v>
+        <v>79.7</v>
       </c>
       <c r="H25" t="n">
-        <v>76</v>
-      </c>
-      <c r="I25" t="n">
-        <v>38.9</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>María</t>
+          <t>Ana</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Fernández</t>
+          <t>López</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>María Fernández</t>
+          <t>Ana López</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>72</v>
+        <v>76.7</v>
       </c>
       <c r="F26" t="n">
-        <v>79.7</v>
+        <v>74.09999999999999</v>
       </c>
       <c r="G26" t="n">
-        <v>95.8</v>
+        <v>89.3</v>
       </c>
       <c r="H26" t="n">
-        <v>82.5</v>
-      </c>
-      <c r="I26" t="n">
-        <v>15.8</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>María</t>
+          <t>Ana</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>García</t>
+          <t>López</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>María García</t>
+          <t>Ana López</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>59.2</v>
+        <v>68.59999999999999</v>
       </c>
       <c r="F27" t="n">
-        <v>67.59999999999999</v>
+        <v>98.09999999999999</v>
       </c>
       <c r="G27" t="n">
-        <v>94.09999999999999</v>
+        <v>66.8</v>
       </c>
       <c r="H27" t="n">
-        <v>73.59999999999999</v>
-      </c>
-      <c r="I27" t="n">
-        <v>87.59999999999999</v>
+        <v>77.8</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Pedro</t>
+          <t>Ana</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Fernández</t>
+          <t>López</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Pedro Fernández</t>
+          <t>Ana López</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>99</v>
+        <v>63.3</v>
       </c>
       <c r="F28" t="n">
-        <v>63.3</v>
+        <v>52.4</v>
       </c>
       <c r="G28" t="n">
-        <v>84.90000000000001</v>
+        <v>93.40000000000001</v>
       </c>
       <c r="H28" t="n">
-        <v>82.40000000000001</v>
-      </c>
-      <c r="I28" t="n">
-        <v>41.6</v>
+        <v>69.7</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Pedro</t>
+          <t>Ana</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>García</t>
+          <t>López</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Pedro García</t>
+          <t>Ana López</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>89.3</v>
+        <v>72.2</v>
       </c>
       <c r="F29" t="n">
-        <v>85.40000000000001</v>
+        <v>75.8</v>
       </c>
       <c r="G29" t="n">
-        <v>78</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="H29" t="n">
-        <v>84.2</v>
-      </c>
-      <c r="I29" t="n">
-        <v>85.59999999999999</v>
+        <v>82.09999999999999</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1471,173 +1382,158 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>González</t>
+          <t>López</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Pedro González</t>
+          <t>Pedro López</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>55.6</v>
+        <v>92.40000000000001</v>
       </c>
       <c r="F30" t="n">
-        <v>78.59999999999999</v>
+        <v>73.3</v>
       </c>
       <c r="G30" t="n">
-        <v>65.59999999999999</v>
+        <v>77.3</v>
       </c>
       <c r="H30" t="n">
-        <v>66.59999999999999</v>
-      </c>
-      <c r="I30" t="n">
-        <v>28.2</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Pedro</t>
+          <t>Sofía</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>López</t>
+          <t>Martínez</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Pedro López</t>
+          <t>Sofía Martínez</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>92.40000000000001</v>
+        <v>79.09999999999999</v>
       </c>
       <c r="F31" t="n">
-        <v>73.3</v>
+        <v>52.6</v>
       </c>
       <c r="G31" t="n">
-        <v>77.3</v>
+        <v>75.09999999999999</v>
       </c>
       <c r="H31" t="n">
-        <v>81</v>
-      </c>
-      <c r="I31" t="n">
-        <v>67.40000000000001</v>
+        <v>68.90000000000001</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Pedro</t>
+          <t>Juan</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Pérez</t>
+          <t>Martínez</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Pedro Pérez</t>
+          <t>Juan Martínez</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>62</v>
+        <v>93.2</v>
       </c>
       <c r="F32" t="n">
-        <v>66.09999999999999</v>
+        <v>70.40000000000001</v>
       </c>
       <c r="G32" t="n">
-        <v>59.9</v>
+        <v>83.7</v>
       </c>
       <c r="H32" t="n">
-        <v>62.7</v>
-      </c>
-      <c r="I32" t="n">
-        <v>65.7</v>
+        <v>82.40000000000001</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Sofía</t>
+          <t>Luis</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>García</t>
+          <t>Martínez</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Sofía García</t>
+          <t>Luis Martínez</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>87</v>
+        <v>93.7</v>
       </c>
       <c r="F33" t="n">
-        <v>62.6</v>
+        <v>84.3</v>
       </c>
       <c r="G33" t="n">
-        <v>58.4</v>
+        <v>51</v>
       </c>
       <c r="H33" t="n">
-        <v>69.3</v>
-      </c>
-      <c r="I33" t="n">
-        <v>91.90000000000001</v>
+        <v>76.3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Sofía</t>
+          <t>Alberto</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>González</t>
+          <t>Martínez</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Sofía González</t>
+          <t>Alberto Martínez</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>59.2</v>
+        <v>76.5</v>
       </c>
       <c r="F34" t="n">
-        <v>95.7</v>
+        <v>86.40000000000001</v>
       </c>
       <c r="G34" t="n">
-        <v>52.9</v>
+        <v>67.40000000000001</v>
       </c>
       <c r="H34" t="n">
-        <v>69.3</v>
-      </c>
-      <c r="I34" t="n">
-        <v>26.9</v>
+        <v>76.8</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1646,37 +1542,34 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>González</t>
+          <t>Martínez</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Sofía González</t>
+          <t>Sofía Martínez</t>
         </is>
       </c>
       <c r="E35" t="n">
         <v>65.59999999999999</v>
       </c>
       <c r="F35" t="n">
-        <v>74.09999999999999</v>
+        <v>73.90000000000001</v>
       </c>
       <c r="G35" t="n">
-        <v>80.90000000000001</v>
+        <v>50.3</v>
       </c>
       <c r="H35" t="n">
-        <v>73.5</v>
-      </c>
-      <c r="I35" t="n">
-        <v>84.90000000000001</v>
+        <v>63.3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Sofía</t>
+          <t>Alberto</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1686,32 +1579,29 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Sofía Martínez</t>
+          <t>Alberto Martínez</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>79.09999999999999</v>
+        <v>92.09999999999999</v>
       </c>
       <c r="F36" t="n">
-        <v>52.6</v>
+        <v>95.09999999999999</v>
       </c>
       <c r="G36" t="n">
-        <v>75.09999999999999</v>
+        <v>63</v>
       </c>
       <c r="H36" t="n">
-        <v>68.90000000000001</v>
-      </c>
-      <c r="I36" t="n">
-        <v>69.90000000000001</v>
+        <v>83.40000000000001</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Sofía</t>
+          <t>Luis</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1721,32 +1611,29 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Sofía Martínez</t>
+          <t>Luis Martínez</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>65.59999999999999</v>
+        <v>50.5</v>
       </c>
       <c r="F37" t="n">
-        <v>73.90000000000001</v>
+        <v>78.2</v>
       </c>
       <c r="G37" t="n">
-        <v>50.3</v>
+        <v>77.09999999999999</v>
       </c>
       <c r="H37" t="n">
-        <v>63.3</v>
-      </c>
-      <c r="I37" t="n">
-        <v>74</v>
+        <v>68.59999999999999</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Sofía</t>
+          <t>Alberto</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1756,163 +1643,148 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Sofía Pérez</t>
+          <t>Alberto Pérez</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>80.90000000000001</v>
+        <v>83.40000000000001</v>
       </c>
       <c r="F38" t="n">
-        <v>64.09999999999999</v>
+        <v>95.90000000000001</v>
       </c>
       <c r="G38" t="n">
-        <v>78.8</v>
+        <v>75.8</v>
       </c>
       <c r="H38" t="n">
-        <v>74.59999999999999</v>
-      </c>
-      <c r="I38" t="n">
-        <v>25.1</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Victor</t>
+          <t>Sofía</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Fernández</t>
+          <t>Pérez</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Victor Fernández</t>
+          <t>Sofía Pérez</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>60.8</v>
+        <v>80.90000000000001</v>
       </c>
       <c r="F39" t="n">
-        <v>80.09999999999999</v>
+        <v>64.09999999999999</v>
       </c>
       <c r="G39" t="n">
-        <v>98.5</v>
+        <v>78.8</v>
       </c>
       <c r="H39" t="n">
-        <v>79.8</v>
-      </c>
-      <c r="I39" t="n">
-        <v>87.5</v>
+        <v>74.59999999999999</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Victor</t>
+          <t>Pedro</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>García</t>
+          <t>Pérez</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Victor García</t>
+          <t>Pedro Pérez</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>67.8</v>
+        <v>62</v>
       </c>
       <c r="F40" t="n">
-        <v>58.6</v>
+        <v>66.09999999999999</v>
       </c>
       <c r="G40" t="n">
-        <v>76.59999999999999</v>
+        <v>59.9</v>
       </c>
       <c r="H40" t="n">
-        <v>67.7</v>
-      </c>
-      <c r="I40" t="n">
-        <v>74.7</v>
+        <v>62.7</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Victor</t>
+          <t>Alberto</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>García</t>
+          <t>Pérez</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Victor García</t>
+          <t>Alberto Pérez</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>60.9</v>
+        <v>53.8</v>
       </c>
       <c r="F41" t="n">
-        <v>70.09999999999999</v>
+        <v>99.3</v>
       </c>
       <c r="G41" t="n">
-        <v>86.3</v>
+        <v>91.59999999999999</v>
       </c>
       <c r="H41" t="n">
-        <v>72.40000000000001</v>
-      </c>
-      <c r="I41" t="n">
-        <v>69.90000000000001</v>
+        <v>81.59999999999999</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Victor</t>
+          <t>Alberto</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>González</t>
+          <t>Pérez</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Victor González</t>
+          <t>Alberto Pérez</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>82.5</v>
+        <v>61.1</v>
       </c>
       <c r="F42" t="n">
-        <v>64.40000000000001</v>
+        <v>60.8</v>
       </c>
       <c r="G42" t="n">
-        <v>79.7</v>
+        <v>70.2</v>
       </c>
       <c r="H42" t="n">
-        <v>75.5</v>
-      </c>
-      <c r="I42" t="n">
-        <v>24.8</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43">
@@ -1946,78 +1818,69 @@
       <c r="H43" t="n">
         <v>70.3</v>
       </c>
-      <c r="I43" t="n">
-        <v>16.5</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Ángel</t>
+          <t>Ana</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Fernández</t>
+          <t>Rodríguez</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Ángel Fernández</t>
+          <t>Ana Rodríguez</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>81.5</v>
+        <v>61.6</v>
       </c>
       <c r="F44" t="n">
-        <v>85</v>
+        <v>63.7</v>
       </c>
       <c r="G44" t="n">
-        <v>96.3</v>
+        <v>69.90000000000001</v>
       </c>
       <c r="H44" t="n">
-        <v>87.59999999999999</v>
-      </c>
-      <c r="I44" t="n">
-        <v>52.5</v>
+        <v>65.09999999999999</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Ángel</t>
+          <t>Alberto</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>González</t>
+          <t>Rodríguez</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Ángel González</t>
+          <t>Alberto Rodríguez</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>74.90000000000001</v>
+        <v>75.09999999999999</v>
       </c>
       <c r="F45" t="n">
-        <v>70.3</v>
+        <v>94</v>
       </c>
       <c r="G45" t="n">
-        <v>83.09999999999999</v>
+        <v>62.9</v>
       </c>
       <c r="H45" t="n">
-        <v>76.09999999999999</v>
-      </c>
-      <c r="I45" t="n">
-        <v>30.6</v>
+        <v>77.3</v>
       </c>
     </row>
     <row r="46">
@@ -2050,9 +1913,6 @@
       </c>
       <c r="H46" t="n">
         <v>85.09999999999999</v>
-      </c>
-      <c r="I46" t="n">
-        <v>8.300000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>